<commit_message>
planning week 11 + logboek toegevoegd
</commit_message>
<xml_diff>
--- a/Logboeken/Logboek Eddie Sprietsma.xlsx
+++ b/Logboeken/Logboek Eddie Sprietsma.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5200" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="5205" yWindow="0" windowWidth="25440" windowHeight="15990" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Gedaan:</t>
   </si>
@@ -49,6 +49,33 @@
   </si>
   <si>
     <t>Aan de analyse werken</t>
+  </si>
+  <si>
+    <t>1 uur</t>
+  </si>
+  <si>
+    <t>Een "GO" gekregen voor ons project</t>
+  </si>
+  <si>
+    <t>0,5 uur</t>
+  </si>
+  <si>
+    <t>Groesgesprek met Robert</t>
+  </si>
+  <si>
+    <t>Uitwerken van de models</t>
+  </si>
+  <si>
+    <t>Tutorials over ASP.NET</t>
+  </si>
+  <si>
+    <t>Models afgemaakt</t>
+  </si>
+  <si>
+    <t>Unit tests afgemaakt</t>
+  </si>
+  <si>
+    <t>Aan de Database gewerkt</t>
   </si>
 </sst>
 </file>
@@ -403,10 +430,15 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -735,16 +767,17 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="3" max="4" width="10.875" customWidth="1"/>
+    <col min="10" max="10" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32" thickTop="1" thickBot="1">
+    <row r="1" spans="1:10" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -758,7 +791,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="22" thickTop="1" thickBot="1">
+    <row r="2" spans="1:10" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -776,7 +809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="19" thickTop="1">
+    <row r="3" spans="1:10" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -794,7 +827,7 @@
         <v>40947</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18">
+    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
@@ -812,7 +845,7 @@
         <v>40947</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="18">
+    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
@@ -830,7 +863,7 @@
         <v>40949</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18">
+    <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>9</v>
       </c>
@@ -841,13 +874,17 @@
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="17"/>
-      <c r="I6" s="18"/>
+      <c r="I6" s="18" t="s">
+        <v>10</v>
+      </c>
       <c r="J6" s="19">
-        <v>40952</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="18">
-      <c r="A7" s="12"/>
+        <v>40949</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
@@ -855,11 +892,17 @@
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
       <c r="H7" s="17"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="20"/>
-    </row>
-    <row r="8" spans="1:10" ht="18">
-      <c r="A8" s="12"/>
+      <c r="I7" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="19">
+        <v>40953</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>13</v>
+      </c>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
@@ -867,11 +910,17 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="17"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="20"/>
-    </row>
-    <row r="9" spans="1:10" ht="18">
-      <c r="A9" s="12"/>
+      <c r="I8" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="19">
+        <v>40953</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
@@ -879,11 +928,17 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="20"/>
-    </row>
-    <row r="10" spans="1:10" ht="18">
-      <c r="A10" s="12"/>
+      <c r="I9" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="19">
+        <v>40955</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
@@ -891,11 +946,17 @@
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="17"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="20"/>
-    </row>
-    <row r="11" spans="1:10" ht="18">
-      <c r="A11" s="12"/>
+      <c r="I10" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="19">
+        <v>40961</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>16</v>
+      </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
@@ -903,11 +964,17 @@
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="17"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="20"/>
-    </row>
-    <row r="12" spans="1:10" ht="18">
-      <c r="A12" s="12"/>
+      <c r="I11" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="19">
+        <v>40961</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>17</v>
+      </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
@@ -915,11 +982,17 @@
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="17"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="20"/>
-    </row>
-    <row r="13" spans="1:10" ht="18">
-      <c r="A13" s="12"/>
+      <c r="I12" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="19">
+        <v>40961</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
@@ -927,11 +1000,17 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
       <c r="H13" s="17"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="20"/>
-    </row>
-    <row r="14" spans="1:10" ht="18">
-      <c r="A14" s="12"/>
+      <c r="I13" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="19">
+        <v>40973</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>13</v>
+      </c>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
@@ -939,10 +1018,14 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
       <c r="H14" s="17"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="20"/>
-    </row>
-    <row r="15" spans="1:10" ht="18">
+      <c r="I14" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="19">
+        <v>40973</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -952,9 +1035,11 @@
       <c r="G15" s="16"/>
       <c r="H15" s="17"/>
       <c r="I15" s="18"/>
-      <c r="J15" s="20"/>
-    </row>
-    <row r="16" spans="1:10" ht="18">
+      <c r="J15" s="19">
+        <v>40980</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -966,7 +1051,7 @@
       <c r="I16" s="18"/>
       <c r="J16" s="20"/>
     </row>
-    <row r="17" spans="1:10" ht="18">
+    <row r="17" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -978,7 +1063,7 @@
       <c r="I17" s="18"/>
       <c r="J17" s="20"/>
     </row>
-    <row r="18" spans="1:10" ht="18">
+    <row r="18" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -990,7 +1075,7 @@
       <c r="I18" s="18"/>
       <c r="J18" s="20"/>
     </row>
-    <row r="19" spans="1:10" ht="18">
+    <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -1002,7 +1087,7 @@
       <c r="I19" s="18"/>
       <c r="J19" s="20"/>
     </row>
-    <row r="20" spans="1:10" ht="18">
+    <row r="20" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -1014,7 +1099,7 @@
       <c r="I20" s="18"/>
       <c r="J20" s="20"/>
     </row>
-    <row r="21" spans="1:10" ht="18">
+    <row r="21" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -1026,7 +1111,7 @@
       <c r="I21" s="18"/>
       <c r="J21" s="20"/>
     </row>
-    <row r="22" spans="1:10" ht="18">
+    <row r="22" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -1038,7 +1123,7 @@
       <c r="I22" s="18"/>
       <c r="J22" s="20"/>
     </row>
-    <row r="23" spans="1:10" ht="18">
+    <row r="23" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -1050,7 +1135,7 @@
       <c r="I23" s="18"/>
       <c r="J23" s="20"/>
     </row>
-    <row r="24" spans="1:10" ht="18">
+    <row r="24" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="12"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
@@ -1062,7 +1147,7 @@
       <c r="I24" s="18"/>
       <c r="J24" s="20"/>
     </row>
-    <row r="25" spans="1:10" ht="18">
+    <row r="25" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="12"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -1074,7 +1159,7 @@
       <c r="I25" s="18"/>
       <c r="J25" s="20"/>
     </row>
-    <row r="26" spans="1:10" ht="18">
+    <row r="26" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="12"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -1086,7 +1171,7 @@
       <c r="I26" s="18"/>
       <c r="J26" s="20"/>
     </row>
-    <row r="27" spans="1:10" ht="18">
+    <row r="27" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="12"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -1098,7 +1183,7 @@
       <c r="I27" s="18"/>
       <c r="J27" s="20"/>
     </row>
-    <row r="28" spans="1:10" ht="18">
+    <row r="28" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -1110,7 +1195,7 @@
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
     </row>
-    <row r="29" spans="1:10" ht="18">
+    <row r="29" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="12"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
@@ -1122,7 +1207,7 @@
       <c r="I29" s="18"/>
       <c r="J29" s="20"/>
     </row>
-    <row r="30" spans="1:10" ht="18">
+    <row r="30" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="12"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
@@ -1134,7 +1219,7 @@
       <c r="I30" s="18"/>
       <c r="J30" s="20"/>
     </row>
-    <row r="31" spans="1:10" ht="18">
+    <row r="31" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="12"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -1146,7 +1231,7 @@
       <c r="I31" s="18"/>
       <c r="J31" s="20"/>
     </row>
-    <row r="32" spans="1:10" ht="18">
+    <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="12"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -1158,7 +1243,7 @@
       <c r="I32" s="18"/>
       <c r="J32" s="20"/>
     </row>
-    <row r="33" spans="1:10" ht="18">
+    <row r="33" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="12"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -1170,7 +1255,7 @@
       <c r="I33" s="18"/>
       <c r="J33" s="20"/>
     </row>
-    <row r="34" spans="1:10" ht="18">
+    <row r="34" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="12"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -1182,7 +1267,7 @@
       <c r="I34" s="18"/>
       <c r="J34" s="20"/>
     </row>
-    <row r="35" spans="1:10" ht="18">
+    <row r="35" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="12"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -1194,7 +1279,7 @@
       <c r="I35" s="18"/>
       <c r="J35" s="20"/>
     </row>
-    <row r="36" spans="1:10" ht="18">
+    <row r="36" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="12"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -1206,7 +1291,7 @@
       <c r="I36" s="18"/>
       <c r="J36" s="20"/>
     </row>
-    <row r="37" spans="1:10" ht="18">
+    <row r="37" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="12"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -1218,7 +1303,7 @@
       <c r="I37" s="18"/>
       <c r="J37" s="20"/>
     </row>
-    <row r="38" spans="1:10" ht="18">
+    <row r="38" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="11"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -1230,7 +1315,7 @@
       <c r="I38" s="18"/>
       <c r="J38" s="20"/>
     </row>
-    <row r="39" spans="1:10" ht="18">
+    <row r="39" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="12"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -1242,7 +1327,7 @@
       <c r="I39" s="18"/>
       <c r="J39" s="20"/>
     </row>
-    <row r="40" spans="1:10" ht="18">
+    <row r="40" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="12"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -1254,7 +1339,7 @@
       <c r="I40" s="18"/>
       <c r="J40" s="20"/>
     </row>
-    <row r="41" spans="1:10" ht="19" thickBot="1">
+    <row r="41" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="21"/>
       <c r="B41" s="22"/>
       <c r="C41" s="22"/>
@@ -1266,7 +1351,7 @@
       <c r="I41" s="24"/>
       <c r="J41" s="25"/>
     </row>
-    <row r="42" spans="1:10" ht="16" thickTop="1"/>
+    <row r="42" spans="1:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
logboek + tagpagina + badgepagina
</commit_message>
<xml_diff>
--- a/Logboeken/Logboek Eddie Sprietsma.xlsx
+++ b/Logboeken/Logboek Eddie Sprietsma.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>Gedaan:</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>Frontpagina: Tags en UnixTimeStamp</t>
+  </si>
+  <si>
+    <t>Vraagpagina</t>
+  </si>
+  <si>
+    <t>Vraagpagina afgemaakt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tagpagina </t>
+  </si>
+  <si>
+    <t>afgemaakt</t>
   </si>
 </sst>
 </file>
@@ -778,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1092,7 +1104,9 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
+      <c r="A18" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -1100,13 +1114,17 @@
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
       <c r="H18" s="17"/>
-      <c r="I18" s="18"/>
+      <c r="I18" s="18" t="s">
+        <v>20</v>
+      </c>
       <c r="J18" s="19">
         <v>40982</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
+      <c r="A19" s="12" t="s">
+        <v>13</v>
+      </c>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
@@ -1114,11 +1132,17 @@
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
       <c r="H19" s="17"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="20"/>
+      <c r="I19" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="19">
+        <v>40987</v>
+      </c>
     </row>
     <row r="20" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
+      <c r="A20" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
@@ -1126,11 +1150,17 @@
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
       <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="20"/>
+      <c r="I20" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="19">
+        <v>40987</v>
+      </c>
     </row>
     <row r="21" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
+      <c r="A21" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -1138,20 +1168,32 @@
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
       <c r="H21" s="17"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="20"/>
+      <c r="I21" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="19">
+        <v>40988</v>
+      </c>
     </row>
     <row r="22" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="16"/>
+      <c r="A22" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
       <c r="H22" s="17"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="20"/>
+      <c r="I22" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" s="19">
+        <v>40989</v>
+      </c>
     </row>
     <row r="23" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>

</xml_diff>